<commit_message>
Add results for V100 and TitanX Pascal
</commit_message>
<xml_diff>
--- a/results/train/DeepBench_NV_TitanX_Pascal.xlsx
+++ b/results/train/DeepBench_NV_TitanX_Pascal.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10319"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patwarymostofa/Documents/mostofa/deepbench-internal/DeepBench-internal/results/train/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharan/Desktop/svail_mnt/DeepBench-ext/results/train/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B0D9AA57-EC6E-1949-8D75-947F19181543}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33340" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33340" windowHeight="19220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results - FP32" sheetId="3" r:id="rId1"/>
     <sheet name="Specs" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="81">
   <si>
     <t>Dense Matrix Multiplication</t>
   </si>
@@ -82,15 +83,6 @@
   </si>
   <si>
     <t>Time Forward (msec)</t>
-  </si>
-  <si>
-    <t>Time Backward (msec)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Forward (msec) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Backward (msec) </t>
   </si>
   <si>
     <t>Forward (msec)</t>
@@ -148,9 +140,6 @@
   </si>
   <si>
     <t>TERAFLOPS FWD</t>
-  </si>
-  <si>
-    <t>TERAFLOPS BWD</t>
   </si>
   <si>
     <t>CPU Model</t>
@@ -269,11 +258,26 @@
   <si>
     <t>Baidu RingAllReduce</t>
   </si>
+  <si>
+    <t>Time Backward wrt Weights (msec)</t>
+  </si>
+  <si>
+    <t>Time Backward wrt Inputs (msec)</t>
+  </si>
+  <si>
+    <t>TERAFLOPS BWD Inputs</t>
+  </si>
+  <si>
+    <t>TERAFLOPS BWD Weights</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -983,6 +987,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1308,11 +1315,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="H380" sqref="H380"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,10 +1328,10 @@
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
     <col min="8" max="8" width="32.6640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="20.83203125" customWidth="1"/>
     <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -1335,10 +1342,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1361,10 +1368,10 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -5567,52 +5574,52 @@
         <v>10</v>
       </c>
       <c r="H174" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I174" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J174" t="s">
+        <v>24</v>
+      </c>
+      <c r="K174" t="s">
+        <v>23</v>
+      </c>
+      <c r="L174" t="s">
+        <v>26</v>
+      </c>
+      <c r="M174" t="s">
+        <v>25</v>
+      </c>
+      <c r="N174" t="s">
+        <v>18</v>
+      </c>
+      <c r="O174" t="s">
+        <v>19</v>
+      </c>
+      <c r="P174" t="s">
+        <v>20</v>
+      </c>
+      <c r="R174" t="s">
         <v>27</v>
       </c>
-      <c r="K174" t="s">
-        <v>26</v>
-      </c>
-      <c r="L174" t="s">
+      <c r="S174" t="s">
+        <v>28</v>
+      </c>
+      <c r="T174" t="s">
+        <v>55</v>
+      </c>
+      <c r="U174" t="s">
+        <v>33</v>
+      </c>
+      <c r="V174" t="s">
+        <v>34</v>
+      </c>
+      <c r="W174" t="s">
+        <v>35</v>
+      </c>
+      <c r="X174" t="s">
         <v>29</v>
-      </c>
-      <c r="M174" t="s">
-        <v>28</v>
-      </c>
-      <c r="N174" t="s">
-        <v>21</v>
-      </c>
-      <c r="O174" t="s">
-        <v>22</v>
-      </c>
-      <c r="P174" t="s">
-        <v>23</v>
-      </c>
-      <c r="R174" t="s">
-        <v>30</v>
-      </c>
-      <c r="S174" t="s">
-        <v>31</v>
-      </c>
-      <c r="T174" t="s">
-        <v>59</v>
-      </c>
-      <c r="U174" t="s">
-        <v>36</v>
-      </c>
-      <c r="V174" t="s">
-        <v>37</v>
-      </c>
-      <c r="W174" t="s">
-        <v>38</v>
-      </c>
-      <c r="X174" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="175" spans="1:31" x14ac:dyDescent="0.2">
@@ -5653,7 +5660,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="O175" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P175" s="2">
         <v>0.28000000000000003</v>
@@ -5675,14 +5682,14 @@
         <v>5.2245333333333326</v>
       </c>
       <c r="V175" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W175" s="2">
         <f t="shared" ref="W175:W206" si="10">(2*$R175*$S175*$F175*$G175*$E175*$I175*$H175)/(P175/1000)/10^12</f>
         <v>2.4629942857142857</v>
       </c>
       <c r="X175" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA175" s="2"/>
       <c r="AE175" s="2"/>
@@ -5725,7 +5732,7 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="O176" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P176" s="2">
         <v>0.51500000000000001</v>
@@ -5747,14 +5754,14 @@
         <v>5.9708952380952383</v>
       </c>
       <c r="V176" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W176" s="2">
         <f t="shared" si="10"/>
         <v>2.6782073786407765</v>
       </c>
       <c r="X176" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA176" s="2"/>
       <c r="AE176" s="2"/>
@@ -5797,7 +5804,7 @@
         <v>0.41</v>
       </c>
       <c r="O177" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P177" s="2">
         <v>0.98699999999999999</v>
@@ -5819,14 +5826,14 @@
         <v>6.7281795121951218</v>
       </c>
       <c r="V177" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W177" s="2">
         <f t="shared" si="10"/>
         <v>2.7948871327254308</v>
       </c>
       <c r="X177" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA177" s="2"/>
       <c r="AE177" s="2"/>
@@ -5869,7 +5876,7 @@
         <v>0.82499999999999996</v>
       </c>
       <c r="O178" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P178" s="2">
         <v>2.1349999999999998</v>
@@ -5891,14 +5898,14 @@
         <v>6.6874026666666673</v>
       </c>
       <c r="V178" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W178" s="2">
         <f t="shared" si="10"/>
         <v>2.5841251522248245</v>
       </c>
       <c r="X178" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA178" s="2"/>
       <c r="AE178" s="2"/>
@@ -5971,7 +5978,7 @@
         <v>5.7289507760532148</v>
       </c>
       <c r="X179" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA179" s="2"/>
       <c r="AE179" s="2"/>
@@ -6044,7 +6051,7 @@
         <v>5.7802165548098428</v>
       </c>
       <c r="X180" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA180" s="2"/>
       <c r="AE180" s="2"/>
@@ -6117,7 +6124,7 @@
         <v>5.9878488991888759</v>
       </c>
       <c r="X181" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA181" s="2"/>
       <c r="AE181" s="2"/>
@@ -6190,7 +6197,7 @@
         <v>6.0687182618907807</v>
       </c>
       <c r="X182" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA182" s="2"/>
       <c r="AE182" s="2"/>
@@ -6233,7 +6240,7 @@
         <v>0.11899999999999999</v>
       </c>
       <c r="O183" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P183" s="2">
         <v>0.40600000000000003</v>
@@ -6255,14 +6262,14 @@
         <v>0.89217075630252107</v>
       </c>
       <c r="V183" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W183" s="2">
         <f t="shared" si="10"/>
         <v>0.26149832512315269</v>
       </c>
       <c r="X183" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA183" s="2"/>
       <c r="AE183" s="2"/>
@@ -6335,7 +6342,7 @@
         <v>1.7158516363636365</v>
       </c>
       <c r="X184" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA184" s="2"/>
       <c r="AE184" s="2"/>
@@ -6408,7 +6415,7 @@
         <v>2.5582727710843374</v>
       </c>
       <c r="X185" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA185" s="2"/>
       <c r="AE185" s="2"/>
@@ -6481,7 +6488,7 @@
         <v>4.6412380327868847</v>
       </c>
       <c r="X186" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA186" s="2"/>
       <c r="AE186" s="2"/>
@@ -6524,7 +6531,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="O187" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P187" s="2">
         <v>0.10199999999999999</v>
@@ -6546,14 +6553,14 @@
         <v>2.1789612972972972</v>
       </c>
       <c r="V187" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W187" s="2">
         <f t="shared" si="10"/>
         <v>0.79040752941176473</v>
       </c>
       <c r="X187" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA187" s="2"/>
       <c r="AE187" s="2"/>
@@ -6626,7 +6633,7 @@
         <v>5.5303112025723467</v>
       </c>
       <c r="X188" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA188" s="2"/>
       <c r="AE188" s="2"/>
@@ -6699,7 +6706,7 @@
         <v>7.3816600171673805</v>
       </c>
       <c r="X189" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA189" s="2"/>
       <c r="AE189" s="2"/>
@@ -6772,7 +6779,7 @@
         <v>6.0447322352941173</v>
       </c>
       <c r="X190" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA190" s="2"/>
       <c r="AE190" s="2"/>
@@ -6845,7 +6852,7 @@
         <v>3.2680001130742049</v>
       </c>
       <c r="X191" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA191" s="2"/>
       <c r="AE191" s="2"/>
@@ -6888,7 +6895,7 @@
         <v>0.39800000000000002</v>
       </c>
       <c r="O192" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P192" s="2">
         <v>1.611</v>
@@ -6910,14 +6917,14 @@
         <v>3.4855930854271353</v>
       </c>
       <c r="V192" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W192" s="2">
         <f t="shared" si="10"/>
         <v>0.86112107262569837</v>
       </c>
       <c r="X192" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA192" s="2"/>
       <c r="AE192" s="2"/>
@@ -6990,7 +6997,7 @@
         <v>8.0116429409853822</v>
       </c>
       <c r="X193" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA193" s="2"/>
       <c r="AE193" s="2"/>
@@ -7064,7 +7071,7 @@
         <v>9.0009151532846712</v>
       </c>
       <c r="X194" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AA194" s="2"/>
       <c r="AE194" s="2"/>
@@ -7138,7 +7145,7 @@
         <v>7.8626485185972372</v>
       </c>
       <c r="X195" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA195" s="2"/>
       <c r="AE195" s="2"/>
@@ -7211,7 +7218,7 @@
         <v>6.0054807272727277</v>
       </c>
       <c r="X196" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA196" s="2"/>
       <c r="AE196" s="2"/>
@@ -7284,7 +7291,7 @@
         <v>3.3448247088607594</v>
       </c>
       <c r="X197" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA197" s="2"/>
       <c r="AE197" s="2"/>
@@ -7327,7 +7334,7 @@
         <v>0.77400000000000002</v>
       </c>
       <c r="O198" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P198" s="2">
         <v>3.198</v>
@@ -7349,14 +7356,14 @@
         <v>3.5846667906976744</v>
       </c>
       <c r="V198" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W198" s="2">
         <f t="shared" si="10"/>
         <v>0.8675835196998124</v>
       </c>
       <c r="X198" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA198" s="2"/>
       <c r="AE198" s="2"/>
@@ -7429,7 +7436,7 @@
         <v>8.5708106064291929</v>
       </c>
       <c r="X199" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA199" s="2"/>
       <c r="AE199" s="2"/>
@@ -7503,7 +7510,7 @@
         <v>9.398224523340744</v>
       </c>
       <c r="X200" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AA200" s="2"/>
       <c r="AE200" s="2"/>
@@ -7577,7 +7584,7 @@
         <v>8.3248970531645572</v>
       </c>
       <c r="X201" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA201" s="2"/>
       <c r="AE201" s="2"/>
@@ -7650,7 +7657,7 @@
         <v>7.8584729219330862</v>
       </c>
       <c r="X202" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA202" s="2"/>
       <c r="AE202" s="2"/>
@@ -7723,7 +7730,7 @@
         <v>2.1470552106790479</v>
       </c>
       <c r="X203" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA203" s="2"/>
       <c r="AE203" s="2"/>
@@ -7766,7 +7773,7 @@
         <v>0.498</v>
       </c>
       <c r="O204" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P204" s="2">
         <v>1.1020000000000001</v>
@@ -7788,14 +7795,14 @@
         <v>7.5832258313253016</v>
       </c>
       <c r="V204" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="W204" s="2">
         <f t="shared" si="10"/>
         <v>3.4269024174228671</v>
       </c>
       <c r="X204" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA204" s="2"/>
       <c r="AE204" s="2"/>
@@ -7868,7 +7875,7 @@
         <v>6.4874020202020199</v>
       </c>
       <c r="X205" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA205" s="2"/>
       <c r="AE205" s="2"/>
@@ -7941,7 +7948,7 @@
         <v>2.0971519999999999</v>
       </c>
       <c r="X206" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA206" s="2"/>
       <c r="AE206" s="2"/>
@@ -8014,7 +8021,7 @@
         <v>3.0754324022346369</v>
       </c>
       <c r="X207" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA207" s="2"/>
       <c r="AE207" s="2"/>
@@ -8087,7 +8094,7 @@
         <v>3.7595285853658535</v>
       </c>
       <c r="X208" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA208" s="2"/>
       <c r="AE208" s="2"/>
@@ -8160,7 +8167,7 @@
         <v>3.3734490505050503</v>
       </c>
       <c r="X209" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA209" s="2"/>
       <c r="AE209" s="2"/>
@@ -8233,7 +8240,7 @@
         <v>5.3247999999999989</v>
       </c>
       <c r="X210" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AA210" s="2"/>
       <c r="AE210" s="2"/>
@@ -8306,7 +8313,7 @@
         <v>5.7089137777777772</v>
       </c>
       <c r="X211" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="212" spans="2:31" x14ac:dyDescent="0.2">
@@ -8377,7 +8384,7 @@
         <v>2.5690111999999998</v>
       </c>
       <c r="X212" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="213" spans="2:31" x14ac:dyDescent="0.2">
@@ -8448,7 +8455,7 @@
         <v>10.754000372093026</v>
       </c>
       <c r="X213" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="214" spans="2:31" x14ac:dyDescent="0.2">
@@ -8520,7 +8527,7 @@
         <v>2.6015303291139245</v>
       </c>
       <c r="X214" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="215" spans="2:31" x14ac:dyDescent="0.2">
@@ -8591,7 +8598,7 @@
         <v>2.6691025454545456</v>
       </c>
       <c r="X215" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216" spans="2:31" x14ac:dyDescent="0.2">
@@ -8662,7 +8669,7 @@
         <v>8.331928216216216</v>
       </c>
       <c r="X216" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="217" spans="2:31" x14ac:dyDescent="0.2">
@@ -8734,7 +8741,7 @@
         <v>2.1408426666666664</v>
       </c>
       <c r="X217" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="218" spans="2:31" x14ac:dyDescent="0.2">
@@ -8806,7 +8813,7 @@
         <v>2.3897778604651165</v>
       </c>
       <c r="X218" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="219" spans="2:31" x14ac:dyDescent="0.2">
@@ -8878,7 +8885,7 @@
         <v>3.877752754716981</v>
       </c>
       <c r="X219" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="220" spans="2:31" x14ac:dyDescent="0.2">
@@ -8949,7 +8956,7 @@
         <v>6.1349521194029855</v>
       </c>
       <c r="X220" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="221" spans="2:31" x14ac:dyDescent="0.2">
@@ -9020,7 +9027,7 @@
         <v>3.236549543307087</v>
       </c>
       <c r="X221" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="222" spans="2:31" x14ac:dyDescent="0.2">
@@ -9091,7 +9098,7 @@
         <v>12.582912</v>
       </c>
       <c r="X222" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="223" spans="2:31" x14ac:dyDescent="0.2">
@@ -9162,7 +9169,7 @@
         <v>3.877752754716981</v>
       </c>
       <c r="X223" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="224" spans="2:31" x14ac:dyDescent="0.2">
@@ -9234,7 +9241,7 @@
         <v>4.8357857882352944</v>
       </c>
       <c r="X224" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="2:24" x14ac:dyDescent="0.2">
@@ -9305,7 +9312,7 @@
         <v>11.669956239747634</v>
       </c>
       <c r="X225" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="226" spans="2:24" x14ac:dyDescent="0.2">
@@ -9376,7 +9383,7 @@
         <v>3.369195016393443</v>
       </c>
       <c r="X226" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="227" spans="2:24" x14ac:dyDescent="0.2">
@@ -9448,7 +9455,7 @@
         <v>3.7367435636363631</v>
       </c>
       <c r="X227" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="228" spans="2:24" x14ac:dyDescent="0.2">
@@ -9520,7 +9527,7 @@
         <v>4.3153993910761157</v>
       </c>
       <c r="X228" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229" spans="2:24" x14ac:dyDescent="0.2">
@@ -9592,7 +9599,7 @@
         <v>0.82013998852553061</v>
       </c>
       <c r="X229" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230" spans="2:24" x14ac:dyDescent="0.2">
@@ -9664,7 +9671,7 @@
         <v>6.2285770318687543</v>
       </c>
       <c r="X230" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="231" spans="2:24" x14ac:dyDescent="0.2">
@@ -9736,7 +9743,7 @@
         <v>8.6911724838772724</v>
       </c>
       <c r="X231" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="232" spans="2:24" x14ac:dyDescent="0.2">
@@ -9808,7 +9815,7 @@
         <v>14.073346399659139</v>
       </c>
       <c r="X232" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="233" spans="2:24" x14ac:dyDescent="0.2">
@@ -9880,7 +9887,7 @@
         <v>9.0672532328939095</v>
       </c>
       <c r="X233" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="234" spans="2:24" x14ac:dyDescent="0.2">
@@ -9952,7 +9959,7 @@
         <v>20.300216542893725</v>
       </c>
       <c r="X234" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="235" spans="2:24" x14ac:dyDescent="0.2">
@@ -10024,7 +10031,7 @@
         <v>8.8238208437856329</v>
       </c>
       <c r="X235" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="236" spans="2:24" x14ac:dyDescent="0.2">
@@ -10096,7 +10103,7 @@
         <v>19.477234791154793</v>
       </c>
       <c r="X236" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="237" spans="2:24" x14ac:dyDescent="0.2">
@@ -10168,7 +10175,7 @@
         <v>1.447330253521127</v>
       </c>
       <c r="X237" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="238" spans="2:24" x14ac:dyDescent="0.2">
@@ -10240,7 +10247,7 @@
         <v>3.0905397894736839</v>
       </c>
       <c r="X238" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="239" spans="2:24" x14ac:dyDescent="0.2">
@@ -10312,7 +10319,7 @@
         <v>2.289926417827298</v>
       </c>
       <c r="X239" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="240" spans="2:24" x14ac:dyDescent="0.2">
@@ -10384,7 +10391,7 @@
         <v>2.8347709793103446</v>
       </c>
       <c r="X240" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241" spans="2:24" x14ac:dyDescent="0.2">
@@ -10456,7 +10463,7 @@
         <v>4.3496485925925921</v>
       </c>
       <c r="X241" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242" spans="2:24" x14ac:dyDescent="0.2">
@@ -10528,7 +10535,7 @@
         <v>4.4198042150537633</v>
       </c>
       <c r="X242" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="243" spans="2:24" x14ac:dyDescent="0.2">
@@ -10600,7 +10607,7 @@
         <v>3.1377236030534346</v>
       </c>
       <c r="X243" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="244" spans="2:24" x14ac:dyDescent="0.2">
@@ -10672,7 +10679,7 @@
         <v>4.6445400225988704</v>
       </c>
       <c r="X244" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="245" spans="2:24" x14ac:dyDescent="0.2">
@@ -10744,7 +10751,7 @@
         <v>4.3381719472295517</v>
       </c>
       <c r="X245" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="246" spans="2:24" x14ac:dyDescent="0.2">
@@ -10816,7 +10823,7 @@
         <v>4.5418982541436463</v>
       </c>
       <c r="X246" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="247" spans="2:24" x14ac:dyDescent="0.2">
@@ -10888,7 +10895,7 @@
         <v>4.6709294545454547</v>
       </c>
       <c r="X247" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="248" spans="2:24" x14ac:dyDescent="0.2">
@@ -10960,7 +10967,7 @@
         <v>2.4911623757575758</v>
       </c>
       <c r="X248" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="249" spans="2:24" x14ac:dyDescent="0.2">
@@ -11032,7 +11039,7 @@
         <v>4.7065854045801521</v>
       </c>
       <c r="X249" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="250" spans="2:24" x14ac:dyDescent="0.2">
@@ -11104,7 +11111,7 @@
         <v>2.9255643558718858</v>
       </c>
       <c r="X250" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="251" spans="2:24" x14ac:dyDescent="0.2">
@@ -11176,7 +11183,7 @@
         <v>2.7773094054054059</v>
       </c>
       <c r="X251" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="252" spans="2:24" x14ac:dyDescent="0.2">
@@ -11248,7 +11255,7 @@
         <v>2.7867240135593221</v>
       </c>
       <c r="X252" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="253" spans="2:24" x14ac:dyDescent="0.2">
@@ -11320,7 +11327,7 @@
         <v>1.458888347826087</v>
       </c>
       <c r="X253" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="254" spans="2:24" x14ac:dyDescent="0.2">
@@ -11392,7 +11399,7 @@
         <v>3.0963600150659136</v>
       </c>
       <c r="X254" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="255" spans="2:24" x14ac:dyDescent="0.2">
@@ -11464,7 +11471,7 @@
         <v>2.3555403553008598</v>
       </c>
       <c r="X255" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="256" spans="2:24" x14ac:dyDescent="0.2">
@@ -11536,7 +11543,7 @@
         <v>3.1139529696969692</v>
       </c>
       <c r="X256" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="257" spans="2:24" x14ac:dyDescent="0.2">
@@ -11608,7 +11615,7 @@
         <v>5.2195783111111114</v>
       </c>
       <c r="X257" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="258" spans="2:24" x14ac:dyDescent="0.2">
@@ -11680,7 +11687,7 @@
         <v>5.303765058064517</v>
       </c>
       <c r="X258" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="259" spans="2:24" x14ac:dyDescent="0.2">
@@ -11752,7 +11759,7 @@
         <v>4.0697207128712867</v>
       </c>
       <c r="X259" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="260" spans="2:24" x14ac:dyDescent="0.2">
@@ -11824,7 +11831,7 @@
         <v>5.728805463414635</v>
       </c>
       <c r="X260" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="261" spans="2:24" x14ac:dyDescent="0.2">
@@ -11896,7 +11903,7 @@
         <v>5.0667709337442215</v>
       </c>
       <c r="X261" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="262" spans="2:24" x14ac:dyDescent="0.2">
@@ -11968,7 +11975,7 @@
         <v>5.390712026229509</v>
       </c>
       <c r="X262" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="263" spans="2:24" x14ac:dyDescent="0.2">
@@ -12040,7 +12047,7 @@
         <v>5.7089137777777781</v>
       </c>
       <c r="X263" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="264" spans="2:24" x14ac:dyDescent="0.2">
@@ -12112,7 +12119,7 @@
         <v>3.3418031869918696</v>
       </c>
       <c r="X264" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="265" spans="2:24" x14ac:dyDescent="0.2">
@@ -12184,7 +12191,7 @@
         <v>8.2391450512249449</v>
       </c>
       <c r="X265" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="266" spans="2:24" x14ac:dyDescent="0.2">
@@ -12256,7 +12263,7 @@
         <v>4.3844457813333326</v>
       </c>
       <c r="X266" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="267" spans="2:24" x14ac:dyDescent="0.2">
@@ -12328,7 +12335,7 @@
         <v>3.9475802352941178</v>
       </c>
       <c r="X267" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="268" spans="2:24" x14ac:dyDescent="0.2">
@@ -12400,18 +12407,18 @@
         <v>4.0697207128712867</v>
       </c>
       <c r="X268" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="271" spans="2:24" x14ac:dyDescent="0.2">
       <c r="D271" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L277" s="3"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>11</v>
       </c>
@@ -12428,16 +12435,25 @@
         <v>17</v>
       </c>
       <c r="H278" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="I278" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="J278" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="K278" t="s">
+        <v>78</v>
+      </c>
+      <c r="L278" t="s">
+        <v>79</v>
+      </c>
+      <c r="M278" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C280">
         <v>1760</v>
       </c>
@@ -12448,21 +12464,32 @@
         <v>50</v>
       </c>
       <c r="G280" s="2">
-        <v>4.32</v>
+        <v>4.516</v>
       </c>
       <c r="H280" s="2">
-        <v>4.0960000000000001</v>
+        <v>3.5459999999999998</v>
       </c>
       <c r="I280" s="2">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="J280" s="2">
         <f>(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(G280/1000)/10^12</f>
-        <v>1.147585185185185</v>
-      </c>
-      <c r="J280" s="2">
+        <v>1.0977785651018599</v>
+      </c>
+      <c r="K280" s="2">
         <f>(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(H280/1000)/10^12</f>
-        <v>1.2103437500000001</v>
-      </c>
-    </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1.3980733220530175</v>
+      </c>
+      <c r="L280" s="2">
+        <f>(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(I280/1000)/10^12</f>
+        <v>7.8442531645569629</v>
+      </c>
+      <c r="M280" s="2">
+        <f>G280+H280+I280</f>
+        <v>8.6939999999999991</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C281">
         <v>1760</v>
       </c>
@@ -12473,21 +12500,32 @@
         <v>50</v>
       </c>
       <c r="G281" s="2">
-        <v>8.7520000000000007</v>
+        <v>10.943</v>
       </c>
       <c r="H281" s="2">
-        <v>9.3390000000000004</v>
+        <v>10.483000000000001</v>
       </c>
       <c r="I281" s="2">
-        <f t="shared" ref="I281:J291" si="28">(2*$E281*$D281*$C281*$C281+$E281*$D281*$C281)/(G281/1000)/10^12</f>
-        <v>1.1328994515539303</v>
+        <v>1.0820000000000001</v>
       </c>
       <c r="J281" s="2">
-        <f t="shared" si="28"/>
-        <v>1.0616914016489989</v>
-      </c>
-    </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+        <f>(2*$E281*$D281*$C281*$C281+$E281*$D281*$C281)/(G281/1000)/10^12</f>
+        <v>0.90607109567760213</v>
+      </c>
+      <c r="K281" s="2">
+        <f>(2*$E281*$D281*$C281*$C281+$E281*$D281*$C281)/(H281/1000)/10^12</f>
+        <v>0.94583001049317927</v>
+      </c>
+      <c r="L281" s="2">
+        <f t="shared" ref="L281:L291" si="28">(2*$E281*$D281*$C281*$C281+$E281*$D281*$C281)/(I281/1000)/10^12</f>
+        <v>9.163711645101662</v>
+      </c>
+      <c r="M281" s="2">
+        <f t="shared" ref="M281:M291" si="29">G281+H281+I281</f>
+        <v>22.508000000000003</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C282">
         <v>1760</v>
       </c>
@@ -12498,21 +12536,32 @@
         <v>50</v>
       </c>
       <c r="G282" s="2">
-        <v>11.506</v>
+        <v>6.1630000000000003</v>
       </c>
       <c r="H282" s="2">
-        <v>11.461</v>
+        <v>5.3550000000000004</v>
       </c>
       <c r="I282" s="2">
+        <v>2.0030000000000001</v>
+      </c>
+      <c r="J282" s="2">
+        <f>(2*$E282*$D282*$C282*$C282+$E282*$D282*$C282)/(G282/1000)/10^12</f>
+        <v>3.217632970955703</v>
+      </c>
+      <c r="K282" s="2">
+        <f>(2*$E282*$D282*$C282*$C282+$E282*$D282*$C282)/(H282/1000)/10^12</f>
+        <v>3.7031320261437903</v>
+      </c>
+      <c r="L282" s="2">
         <f t="shared" si="28"/>
-        <v>1.7234722753346079</v>
-      </c>
-      <c r="J282" s="2">
-        <f t="shared" si="28"/>
-        <v>1.7302392461390803</v>
-      </c>
-    </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9.900285571642538</v>
+      </c>
+      <c r="M282" s="2">
+        <f t="shared" si="29"/>
+        <v>13.521000000000001</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283">
         <f>2560*2560/1760/1760</f>
         <v>2.115702479338843</v>
@@ -12527,21 +12576,32 @@
         <v>50</v>
       </c>
       <c r="G283" s="2">
-        <v>12.007999999999999</v>
+        <v>6.9530000000000003</v>
       </c>
       <c r="H283" s="2">
-        <v>10.028</v>
+        <v>6.3730000000000002</v>
       </c>
       <c r="I283" s="2">
+        <v>4.0140000000000002</v>
+      </c>
+      <c r="J283" s="2">
+        <f>(2*$E283*$D283*$C283*$C283+$E283*$D283*$C283)/(G283/1000)/10^12</f>
+        <v>5.7040908960161083</v>
+      </c>
+      <c r="K283" s="2">
+        <f>(2*$E283*$D283*$C283*$C283+$E283*$D283*$C283)/(H283/1000)/10^12</f>
+        <v>6.2232141848423037</v>
+      </c>
+      <c r="L283" s="2">
         <f t="shared" si="28"/>
-        <v>3.3028434377081948</v>
-      </c>
-      <c r="J283" s="2">
-        <f t="shared" si="28"/>
-        <v>3.9549804547267646</v>
-      </c>
-    </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9.8805540607872437</v>
+      </c>
+      <c r="M283" s="2">
+        <f t="shared" si="29"/>
+        <v>17.34</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C284">
         <v>2048</v>
       </c>
@@ -12552,21 +12612,32 @@
         <v>50</v>
       </c>
       <c r="G284" s="2">
-        <v>6.7720000000000002</v>
+        <v>6.859</v>
       </c>
       <c r="H284" s="2">
-        <v>6.7670000000000003</v>
+        <v>5.6710000000000003</v>
       </c>
       <c r="I284" s="2">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="J284" s="2">
+        <f>(2*$E284*$D284*$C284*$C284+$E284*$D284*$C284)/(G284/1000)/10^12</f>
+        <v>0.97864481702872141</v>
+      </c>
+      <c r="K284" s="2">
+        <f>(2*$E284*$D284*$C284*$C284+$E284*$D284*$C284)/(H284/1000)/10^12</f>
+        <v>1.1836580497266795</v>
+      </c>
+      <c r="L284" s="2">
         <f t="shared" si="28"/>
-        <v>0.99121748375664498</v>
-      </c>
-      <c r="J284" s="2">
-        <f t="shared" si="28"/>
-        <v>0.99194987439042404</v>
-      </c>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
+        <v>8.4647223203026467</v>
+      </c>
+      <c r="M284" s="2">
+        <f t="shared" si="29"/>
+        <v>13.323</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C285">
         <v>2048</v>
       </c>
@@ -12577,21 +12648,32 @@
         <v>50</v>
       </c>
       <c r="G285" s="2">
-        <v>10.119</v>
+        <v>12.414999999999999</v>
       </c>
       <c r="H285" s="2">
-        <v>9.9939999999999998</v>
+        <v>11.92</v>
       </c>
       <c r="I285" s="2">
+        <v>1.381</v>
+      </c>
+      <c r="J285" s="2">
+        <f>(2*$E285*$D285*$C285*$C285+$E285*$D285*$C285)/(G285/1000)/10^12</f>
+        <v>1.0813571969391864</v>
+      </c>
+      <c r="K285" s="2">
+        <f>(2*$E285*$D285*$C285*$C285+$E285*$D285*$C285)/(H285/1000)/10^12</f>
+        <v>1.1262625503355705</v>
+      </c>
+      <c r="L285" s="2">
         <f t="shared" si="28"/>
-        <v>1.3267170273742466</v>
-      </c>
-      <c r="J285" s="2">
-        <f t="shared" si="28"/>
-        <v>1.3433109465679409</v>
-      </c>
-    </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9.7212524257784221</v>
+      </c>
+      <c r="M285" s="2">
+        <f t="shared" si="29"/>
+        <v>25.716000000000001</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C286">
         <v>2048</v>
       </c>
@@ -12602,21 +12684,32 @@
         <v>50</v>
       </c>
       <c r="G286" s="2">
-        <v>15.912000000000001</v>
+        <v>11.162000000000001</v>
       </c>
       <c r="H286" s="2">
-        <v>15.396000000000001</v>
+        <v>10.009</v>
       </c>
       <c r="I286" s="2">
+        <v>2.5739999999999998</v>
+      </c>
+      <c r="J286" s="2">
+        <f>(2*$E286*$D286*$C286*$C286+$E286*$D286*$C286)/(G286/1000)/10^12</f>
+        <v>2.4054917756674428</v>
+      </c>
+      <c r="K286" s="2">
+        <f>(2*$E286*$D286*$C286*$C286+$E286*$D286*$C286)/(H286/1000)/10^12</f>
+        <v>2.6825955839744227</v>
+      </c>
+      <c r="L286" s="2">
         <f t="shared" si="28"/>
-        <v>1.6874119658119655</v>
-      </c>
-      <c r="J286" s="2">
-        <f t="shared" si="28"/>
-        <v>1.743965913224214</v>
-      </c>
-    </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10.431273970473971</v>
+      </c>
+      <c r="M286" s="2">
+        <f t="shared" si="29"/>
+        <v>23.744999999999997</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A287">
         <f>2560*2560/2048/2048</f>
         <v>1.5625</v>
@@ -12631,21 +12724,32 @@
         <v>50</v>
       </c>
       <c r="G287" s="2">
-        <v>14.18</v>
+        <v>9.4190000000000005</v>
       </c>
       <c r="H287" s="2">
-        <v>11.316000000000001</v>
+        <v>8.9990000000000006</v>
       </c>
       <c r="I287" s="2">
+        <v>5.016</v>
+      </c>
+      <c r="J287" s="2">
+        <f>(2*$E287*$D287*$C287*$C287+$E287*$D287*$C287)/(G287/1000)/10^12</f>
+        <v>5.7012632338889473</v>
+      </c>
+      <c r="K287" s="2">
+        <f>(2*$E287*$D287*$C287*$C287+$E287*$D287*$C287)/(H287/1000)/10^12</f>
+        <v>5.9673517501944655</v>
+      </c>
+      <c r="L287" s="2">
         <f t="shared" si="28"/>
-        <v>3.787037968970381</v>
-      </c>
-      <c r="J287" s="2">
-        <f t="shared" si="28"/>
-        <v>4.7455106398020499</v>
-      </c>
-    </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10.705781180223287</v>
+      </c>
+      <c r="M287" s="2">
+        <f t="shared" si="29"/>
+        <v>23.433999999999997</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C288">
         <v>2560</v>
       </c>
@@ -12656,21 +12760,32 @@
         <v>50</v>
       </c>
       <c r="G288" s="2">
-        <v>10.563000000000001</v>
+        <v>10.526999999999999</v>
       </c>
       <c r="H288" s="2">
-        <v>10.288</v>
+        <v>9.3870000000000005</v>
       </c>
       <c r="I288" s="2">
+        <v>1.256</v>
+      </c>
+      <c r="J288" s="2">
+        <f>(2*$E288*$D288*$C288*$C288+$E288*$D288*$C288)/(G288/1000)/10^12</f>
+        <v>0.99627700199487035</v>
+      </c>
+      <c r="K288" s="2">
+        <f>(2*$E288*$D288*$C288*$C288+$E288*$D288*$C288)/(H288/1000)/10^12</f>
+        <v>1.1172694151486096</v>
+      </c>
+      <c r="L288" s="2">
         <f t="shared" si="28"/>
-        <v>0.99288156773643832</v>
-      </c>
-      <c r="J288" s="2">
-        <f t="shared" si="28"/>
-        <v>1.0194214618973561</v>
-      </c>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8.3501656050955422</v>
+      </c>
+      <c r="M288" s="2">
+        <f t="shared" si="29"/>
+        <v>21.17</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C289">
         <v>2560</v>
       </c>
@@ -12681,21 +12796,32 @@
         <v>50</v>
       </c>
       <c r="G289" s="2">
-        <v>12.906000000000001</v>
+        <v>15.121</v>
       </c>
       <c r="H289" s="2">
-        <v>12.74</v>
+        <v>14.598000000000001</v>
       </c>
       <c r="I289" s="2">
+        <v>2.2210000000000001</v>
+      </c>
+      <c r="J289" s="2">
+        <f>(2*$E289*$D289*$C289*$C289+$E289*$D289*$C289)/(G289/1000)/10^12</f>
+        <v>1.3871844454731828</v>
+      </c>
+      <c r="K289" s="2">
+        <f>(2*$E289*$D289*$C289*$C289+$E289*$D289*$C289)/(H289/1000)/10^12</f>
+        <v>1.4368828606658446</v>
+      </c>
+      <c r="L289" s="2">
         <f t="shared" si="28"/>
-        <v>1.6252608089260807</v>
-      </c>
-      <c r="J289" s="2">
-        <f t="shared" si="28"/>
-        <v>1.6464376766091051</v>
-      </c>
-    </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9.4442215218370116</v>
+      </c>
+      <c r="M289" s="2">
+        <f t="shared" si="29"/>
+        <v>31.94</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C290">
         <v>2560</v>
       </c>
@@ -12706,21 +12832,32 @@
         <v>50</v>
       </c>
       <c r="G290" s="2">
-        <v>18.486999999999998</v>
+        <v>16.381</v>
       </c>
       <c r="H290" s="2">
-        <v>18.085000000000001</v>
+        <v>15.938000000000001</v>
       </c>
       <c r="I290" s="2">
+        <v>4.0990000000000002</v>
+      </c>
+      <c r="J290" s="2">
+        <f>(2*$E290*$D290*$C290*$C290+$E290*$D290*$C290)/(G290/1000)/10^12</f>
+        <v>2.5609689274159089</v>
+      </c>
+      <c r="K290" s="2">
+        <f>(2*$E290*$D290*$C290*$C290+$E290*$D290*$C290)/(H290/1000)/10^12</f>
+        <v>2.6321515874011792</v>
+      </c>
+      <c r="L290" s="2">
         <f t="shared" si="28"/>
-        <v>2.2692287553415915</v>
-      </c>
-      <c r="J290" s="2">
-        <f t="shared" si="28"/>
-        <v>2.3196700027647221</v>
-      </c>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+        <v>10.234504025372042</v>
+      </c>
+      <c r="M290" s="2">
+        <f t="shared" si="29"/>
+        <v>36.418000000000006</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C291">
         <v>2560</v>
       </c>
@@ -12731,21 +12868,32 @@
         <v>50</v>
       </c>
       <c r="G291" s="2">
-        <v>16.983000000000001</v>
+        <v>17.024000000000001</v>
       </c>
       <c r="H291" s="2">
-        <v>14.29</v>
+        <v>16.341000000000001</v>
       </c>
       <c r="I291" s="2">
+        <v>7.95</v>
+      </c>
+      <c r="J291" s="2">
+        <f>(2*$E291*$D291*$C291*$C291+$E291*$D291*$C291)/(G291/1000)/10^12</f>
+        <v>4.9284812030075189</v>
+      </c>
+      <c r="K291" s="2">
+        <f>(2*$E291*$D291*$C291*$C291+$E291*$D291*$C291)/(H291/1000)/10^12</f>
+        <v>5.1344754910960155</v>
+      </c>
+      <c r="L291" s="2">
         <f t="shared" si="28"/>
-        <v>4.9403794382617914</v>
-      </c>
-      <c r="J291" s="2">
-        <f t="shared" si="28"/>
-        <v>5.8714110566829953</v>
-      </c>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+        <v>10.553769056603773</v>
+      </c>
+      <c r="M291" s="2">
+        <f t="shared" si="29"/>
+        <v>41.315000000000005</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>12</v>
       </c>
@@ -12759,19 +12907,28 @@
         <v>14</v>
       </c>
       <c r="G295" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H295" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="I295" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="J295" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="K295" t="s">
+        <v>78</v>
+      </c>
+      <c r="L295" t="s">
+        <v>79</v>
+      </c>
+      <c r="M295" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C296">
         <v>512</v>
       </c>
@@ -12782,21 +12939,32 @@
         <v>25</v>
       </c>
       <c r="G296" s="2">
-        <v>1.5589999999999999</v>
+        <v>1.3220000000000001</v>
       </c>
       <c r="H296" s="2">
-        <v>1.9359999999999999</v>
+        <v>1.401</v>
       </c>
       <c r="I296" s="2">
-        <f t="shared" ref="I296:J312" si="29">(8*$E296*$D296*$C296*$C296)/(G296/1000)/10^12</f>
-        <v>0.53807620269403467</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="J296" s="2">
-        <f t="shared" ref="J296:J311" si="30">(8*$E296*$D296*$C296*$C296)/(H296/1000)/10^12</f>
-        <v>0.43329586776859502</v>
-      </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+        <f>(8*$E296*$D296*$C296*$C296)/(G296/1000)/10^12</f>
+        <v>0.63453918305597579</v>
+      </c>
+      <c r="K296" s="2">
+        <f>(8*$E296*$D296*$C296*$C296)/(H296/1000)/10^12</f>
+        <v>0.59875860099928613</v>
+      </c>
+      <c r="L296" s="2">
+        <f>(8*$E296*$D296*$C296*$C296)/(I296/1000)/10^12</f>
+        <v>4.8489063583815035</v>
+      </c>
+      <c r="M296" s="2">
+        <f t="shared" ref="M296:M317" si="30">G296+H296+I296</f>
+        <v>2.8959999999999999</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C297">
         <v>512</v>
       </c>
@@ -12807,21 +12975,32 @@
         <v>25</v>
       </c>
       <c r="G297" s="2">
-        <v>2.7610000000000001</v>
+        <v>2.4119999999999999</v>
       </c>
       <c r="H297" s="2">
-        <v>3.9689999999999999</v>
+        <v>5.7619999999999996</v>
       </c>
       <c r="I297" s="2">
-        <f t="shared" si="29"/>
-        <v>0.60764998189061936</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="J297" s="2">
+        <f>(8*$E297*$D297*$C297*$C297)/(G297/1000)/10^12</f>
+        <v>0.69557280265339971</v>
+      </c>
+      <c r="K297" s="2">
+        <f>(8*$E297*$D297*$C297*$C297)/(H297/1000)/10^12</f>
+        <v>0.29117001041305102</v>
+      </c>
+      <c r="L297" s="2">
+        <f t="shared" ref="L297:L317" si="31">(8*$E297*$D297*$C297*$C297)/(I297/1000)/10^12</f>
+        <v>6.4280521072796937</v>
+      </c>
+      <c r="M297" s="2">
         <f t="shared" si="30"/>
-        <v>0.42270637440161257</v>
-      </c>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8.4349999999999987</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C298">
         <v>512</v>
       </c>
@@ -12832,21 +13011,32 @@
         <v>25</v>
       </c>
       <c r="G298" s="2">
-        <v>2.347</v>
+        <v>2.09</v>
       </c>
       <c r="H298" s="2">
-        <v>3.992</v>
+        <v>2.1680000000000001</v>
       </c>
       <c r="I298" s="2">
-        <f t="shared" si="29"/>
-        <v>1.4296732850447378</v>
+        <v>0.442</v>
       </c>
       <c r="J298" s="2">
+        <f>(8*$E298*$D298*$C298*$C298)/(G298/1000)/10^12</f>
+        <v>1.6054752153110048</v>
+      </c>
+      <c r="K298" s="2">
+        <f>(8*$E298*$D298*$C298*$C298)/(H298/1000)/10^12</f>
+        <v>1.5477136531365312</v>
+      </c>
+      <c r="L298" s="2">
+        <f t="shared" si="31"/>
+        <v>7.5915004524886873</v>
+      </c>
+      <c r="M298" s="2">
         <f t="shared" si="30"/>
-        <v>0.84054188376753503</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C299">
         <v>512</v>
       </c>
@@ -12857,21 +13047,32 @@
         <v>25</v>
       </c>
       <c r="G299" s="2">
-        <v>2.67</v>
+        <v>2.403</v>
       </c>
       <c r="H299" s="2">
-        <v>4.9889999999999999</v>
+        <v>2.5489999999999999</v>
       </c>
       <c r="I299" s="2">
-        <f t="shared" si="29"/>
-        <v>2.5134405992509361</v>
+        <v>0.76</v>
       </c>
       <c r="J299" s="2">
+        <f>(8*$E299*$D299*$C299*$C299)/(G299/1000)/10^12</f>
+        <v>2.7927117769454846</v>
+      </c>
+      <c r="K299" s="2">
+        <f>(8*$E299*$D299*$C299*$C299)/(H299/1000)/10^12</f>
+        <v>2.6327526088662223</v>
+      </c>
+      <c r="L299" s="2">
+        <f t="shared" si="31"/>
+        <v>8.8301136842105254</v>
+      </c>
+      <c r="M299" s="2">
         <f t="shared" si="30"/>
-        <v>1.3451365804770496</v>
-      </c>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5.7119999999999997</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C300">
         <v>1024</v>
       </c>
@@ -12882,21 +13083,32 @@
         <v>25</v>
       </c>
       <c r="G300" s="2">
-        <v>4.6369999999999996</v>
+        <v>4.1920000000000002</v>
       </c>
       <c r="H300" s="2">
-        <v>2.855</v>
+        <v>2.4470000000000001</v>
       </c>
       <c r="I300" s="2">
-        <f t="shared" si="29"/>
-        <v>0.72362372223420324</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="J300" s="2">
+        <f>(8*$E300*$D300*$C300*$C300)/(G300/1000)/10^12</f>
+        <v>0.80043969465648857</v>
+      </c>
+      <c r="K300" s="2">
+        <f>(8*$E300*$D300*$C300*$C300)/(H300/1000)/10^12</f>
+        <v>1.3712477319166325</v>
+      </c>
+      <c r="L300" s="2">
+        <f t="shared" si="31"/>
+        <v>6.3913203809523802</v>
+      </c>
+      <c r="M300" s="2">
         <f t="shared" si="30"/>
-        <v>1.1752865849387042</v>
-      </c>
-    </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
+        <v>7.1640000000000006</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C301">
         <v>1024</v>
       </c>
@@ -12907,21 +13119,32 @@
         <v>25</v>
       </c>
       <c r="G301" s="2">
-        <v>4.5620000000000003</v>
+        <v>4.1660000000000004</v>
       </c>
       <c r="H301" s="2">
-        <v>5.173</v>
+        <v>10.8</v>
       </c>
       <c r="I301" s="2">
-        <f t="shared" si="29"/>
-        <v>1.4710404208680403</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="J301" s="2">
+        <f>(8*$E301*$D301*$C301*$C301)/(G301/1000)/10^12</f>
+        <v>1.6108704752760439</v>
+      </c>
+      <c r="K301" s="2">
+        <f>(8*$E301*$D301*$C301*$C301)/(H301/1000)/10^12</f>
+        <v>0.62137837037037036</v>
+      </c>
+      <c r="L301" s="2">
+        <f t="shared" si="31"/>
+        <v>8.0177854241338107</v>
+      </c>
+      <c r="M301" s="2">
         <f t="shared" si="30"/>
-        <v>1.2972910110187512</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15.803000000000001</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C302">
         <v>1024</v>
       </c>
@@ -12932,21 +13155,32 @@
         <v>25</v>
       </c>
       <c r="G302" s="2">
-        <v>4.359</v>
+        <v>4.4909999999999997</v>
       </c>
       <c r="H302" s="2">
-        <v>8.1389999999999993</v>
+        <v>3.504</v>
       </c>
       <c r="I302" s="2">
-        <f t="shared" si="29"/>
-        <v>3.0790944712089927</v>
+        <v>1.4550000000000001</v>
       </c>
       <c r="J302" s="2">
+        <f>(8*$E302*$D302*$C302*$C302)/(G302/1000)/10^12</f>
+        <v>2.9885933645067921</v>
+      </c>
+      <c r="K302" s="2">
+        <f>(8*$E302*$D302*$C302*$C302)/(H302/1000)/10^12</f>
+        <v>3.830414611872146</v>
+      </c>
+      <c r="L302" s="2">
+        <f t="shared" si="31"/>
+        <v>9.2245861168384859</v>
+      </c>
+      <c r="M302" s="2">
         <f t="shared" si="30"/>
-        <v>1.6490690256788305</v>
-      </c>
-    </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9.4499999999999993</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C303">
         <v>1024</v>
       </c>
@@ -12957,21 +13191,32 @@
         <v>25</v>
       </c>
       <c r="G303" s="2">
-        <v>5.1719999999999997</v>
+        <v>5.6029999999999998</v>
       </c>
       <c r="H303" s="2">
-        <v>11.946999999999999</v>
+        <v>4.734</v>
       </c>
       <c r="I303" s="2">
-        <f t="shared" si="29"/>
-        <v>5.1901673627223515</v>
+        <v>2.6909999999999998</v>
       </c>
       <c r="J303" s="2">
+        <f>(8*$E303*$D303*$C303*$C303)/(G303/1000)/10^12</f>
+        <v>4.7909237194360168</v>
+      </c>
+      <c r="K303" s="2">
+        <f>(8*$E303*$D303*$C303*$C303)/(H303/1000)/10^12</f>
+        <v>5.67037296155471</v>
+      </c>
+      <c r="L303" s="2">
+        <f t="shared" si="31"/>
+        <v>9.9753049424005962</v>
+      </c>
+      <c r="M303" s="2">
         <f t="shared" si="30"/>
-        <v>2.2468858793002426</v>
-      </c>
-    </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13.027999999999999</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C304">
         <v>2048</v>
       </c>
@@ -12982,21 +13227,32 @@
         <v>25</v>
       </c>
       <c r="G304" s="2">
-        <v>20.658000000000001</v>
+        <v>20.073</v>
       </c>
       <c r="H304" s="2">
-        <v>9.8409999999999993</v>
+        <v>9.4949999999999992</v>
       </c>
       <c r="I304" s="2">
-        <f t="shared" si="29"/>
-        <v>0.64971307967857483</v>
+        <v>1.784</v>
       </c>
       <c r="J304" s="2">
+        <f>(8*$E304*$D304*$C304*$C304)/(G304/1000)/10^12</f>
+        <v>0.66864807452797292</v>
+      </c>
+      <c r="K304" s="2">
+        <f>(8*$E304*$D304*$C304*$C304)/(H304/1000)/10^12</f>
+        <v>1.4135621695629279</v>
+      </c>
+      <c r="L304" s="2">
+        <f t="shared" si="31"/>
+        <v>7.5234152466367714</v>
+      </c>
+      <c r="M304" s="2">
         <f t="shared" si="30"/>
-        <v>1.3638626968803984</v>
-      </c>
-    </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
+        <v>31.351999999999997</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C305">
         <v>2048</v>
       </c>
@@ -13007,21 +13263,32 @@
         <v>25</v>
       </c>
       <c r="G305" s="2">
-        <v>13.087999999999999</v>
+        <v>8.1739999999999995</v>
       </c>
       <c r="H305" s="2">
-        <v>11.788</v>
+        <v>20.907</v>
       </c>
       <c r="I305" s="2">
-        <f t="shared" si="29"/>
-        <v>2.0510044009779955</v>
+        <v>2.895</v>
       </c>
       <c r="J305" s="2">
+        <f>(8*$E305*$D305*$C305*$C305)/(G305/1000)/10^12</f>
+        <v>3.2840158551504777</v>
+      </c>
+      <c r="K305" s="2">
+        <f>(8*$E305*$D305*$C305*$C305)/(H305/1000)/10^12</f>
+        <v>1.2839501411010668</v>
+      </c>
+      <c r="L305" s="2">
+        <f t="shared" si="31"/>
+        <v>9.2723818998272893</v>
+      </c>
+      <c r="M305" s="2">
         <f t="shared" si="30"/>
-        <v>2.2771925347811335</v>
-      </c>
-    </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
+        <v>31.975999999999999</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C306">
         <v>2048</v>
       </c>
@@ -13032,21 +13299,32 @@
         <v>25</v>
       </c>
       <c r="G306" s="2">
-        <v>10.186999999999999</v>
+        <v>11.02</v>
       </c>
       <c r="H306" s="2">
-        <v>19.222999999999999</v>
+        <v>21.306999999999999</v>
       </c>
       <c r="I306" s="2">
-        <f t="shared" si="29"/>
-        <v>5.2701571807205267</v>
+        <v>5.2450000000000001</v>
       </c>
       <c r="J306" s="2">
+        <f>(8*$E306*$D306*$C306*$C306)/(G306/1000)/10^12</f>
+        <v>4.8717868602540833</v>
+      </c>
+      <c r="K306" s="2">
+        <f>(8*$E306*$D306*$C306*$C306)/(H306/1000)/10^12</f>
+        <v>2.5196926456094242</v>
+      </c>
+      <c r="L306" s="2">
+        <f t="shared" si="31"/>
+        <v>10.23586104861773</v>
+      </c>
+      <c r="M306" s="2">
         <f t="shared" si="30"/>
-        <v>2.7928570566508868</v>
-      </c>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
+        <v>37.571999999999996</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C307">
         <v>2048</v>
       </c>
@@ -13057,21 +13335,32 @@
         <v>25</v>
       </c>
       <c r="G307" s="2">
-        <v>16.128</v>
+        <v>16.521999999999998</v>
       </c>
       <c r="H307" s="2">
-        <v>19.62</v>
+        <v>13.784000000000001</v>
       </c>
       <c r="I307" s="2">
-        <f t="shared" si="29"/>
-        <v>6.6576253968253969</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="J307" s="2">
+        <f>(8*$E307*$D307*$C307*$C307)/(G307/1000)/10^12</f>
+        <v>6.4988610579832962</v>
+      </c>
+      <c r="K307" s="2">
+        <f>(8*$E307*$D307*$C307*$C307)/(H307/1000)/10^12</f>
+        <v>7.7897694718514208</v>
+      </c>
+      <c r="L307" s="2">
+        <f t="shared" si="31"/>
+        <v>10.694639681274902</v>
+      </c>
+      <c r="M307" s="2">
         <f t="shared" si="30"/>
-        <v>5.472690234454638</v>
-      </c>
-    </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
+        <v>40.345999999999997</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C308">
         <v>4096</v>
       </c>
@@ -13082,21 +13371,32 @@
         <v>25</v>
       </c>
       <c r="G308" s="2">
-        <v>80.944999999999993</v>
+        <v>78.269000000000005</v>
       </c>
       <c r="H308" s="2">
-        <v>57.247999999999998</v>
+        <v>57.773000000000003</v>
       </c>
       <c r="I308" s="2">
-        <f t="shared" si="29"/>
-        <v>0.66325395268392129</v>
+        <v>6.657</v>
       </c>
       <c r="J308" s="2">
+        <f>(8*$E308*$D308*$C308*$C308)/(G308/1000)/10^12</f>
+        <v>0.68593046033550953</v>
+      </c>
+      <c r="K308" s="2">
+        <f>(8*$E308*$D308*$C308*$C308)/(H308/1000)/10^12</f>
+        <v>0.92927649940283519</v>
+      </c>
+      <c r="L308" s="2">
+        <f t="shared" si="31"/>
+        <v>8.064757578488809</v>
+      </c>
+      <c r="M308" s="2">
         <f t="shared" si="30"/>
-        <v>0.93779854667411966</v>
-      </c>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
+        <v>142.69900000000001</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C309">
         <v>4096</v>
       </c>
@@ -13107,21 +13407,32 @@
         <v>25</v>
       </c>
       <c r="G309" s="2">
-        <v>39.863</v>
+        <v>23.702999999999999</v>
       </c>
       <c r="H309" s="2">
-        <v>36.305</v>
+        <v>48.731000000000002</v>
       </c>
       <c r="I309" s="2">
-        <f t="shared" si="29"/>
-        <v>2.6935800717457292</v>
+        <v>11.257</v>
       </c>
       <c r="J309" s="2">
+        <f>(8*$E309*$D309*$C309*$C309)/(G309/1000)/10^12</f>
+        <v>4.52998280386449</v>
+      </c>
+      <c r="K309" s="2">
+        <f>(8*$E309*$D309*$C309*$C309)/(H309/1000)/10^12</f>
+        <v>2.2034060946830558</v>
+      </c>
+      <c r="L309" s="2">
+        <f t="shared" si="31"/>
+        <v>9.5384367415830162</v>
+      </c>
+      <c r="M309" s="2">
         <f t="shared" si="30"/>
-        <v>2.957559080016527</v>
-      </c>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
+        <v>83.691000000000003</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C310">
         <v>4096</v>
       </c>
@@ -13132,21 +13443,32 @@
         <v>25</v>
       </c>
       <c r="G310" s="2">
-        <v>32.213999999999999</v>
+        <v>47.393999999999998</v>
       </c>
       <c r="H310" s="2">
-        <v>46.113</v>
+        <v>52.892000000000003</v>
       </c>
       <c r="I310" s="2">
-        <f t="shared" si="29"/>
-        <v>6.666305482088533</v>
+        <v>20.782</v>
       </c>
       <c r="J310" s="2">
+        <f>(8*$E310*$D310*$C310*$C310)/(G310/1000)/10^12</f>
+        <v>4.5311297801409465</v>
+      </c>
+      <c r="K310" s="2">
+        <f>(8*$E310*$D310*$C310*$C310)/(H310/1000)/10^12</f>
+        <v>4.0601294108749899</v>
+      </c>
+      <c r="L310" s="2">
+        <f t="shared" si="31"/>
+        <v>10.333382966028294</v>
+      </c>
+      <c r="M310" s="2">
         <f t="shared" si="30"/>
-        <v>4.6570026847093011</v>
-      </c>
-    </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
+        <v>121.068</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C311">
         <v>4096</v>
       </c>
@@ -13157,21 +13479,32 @@
         <v>25</v>
       </c>
       <c r="G311" s="2">
-        <v>54.881999999999998</v>
+        <v>52.686999999999998</v>
       </c>
       <c r="H311" s="2">
-        <v>59.124000000000002</v>
+        <v>69.744</v>
       </c>
       <c r="I311" s="2">
-        <f t="shared" si="29"/>
-        <v>7.825821391348712</v>
+        <v>43.350999999999999</v>
       </c>
       <c r="J311" s="2">
+        <f>(8*$E311*$D311*$C311*$C311)/(G311/1000)/10^12</f>
+        <v>8.1518539601799311</v>
+      </c>
+      <c r="K311" s="2">
+        <f>(8*$E311*$D311*$C311*$C311)/(H311/1000)/10^12</f>
+        <v>6.1581889424179854</v>
+      </c>
+      <c r="L311" s="2">
+        <f t="shared" si="31"/>
+        <v>9.9074238102927268</v>
+      </c>
+      <c r="M311" s="2">
         <f t="shared" si="30"/>
-        <v>7.2643381638590077</v>
-      </c>
-    </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
+        <v>165.78199999999998</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C312">
         <v>1536</v>
       </c>
@@ -13182,21 +13515,32 @@
         <v>50</v>
       </c>
       <c r="G312" s="2">
-        <v>11.853999999999999</v>
+        <v>11.811</v>
       </c>
       <c r="H312" s="2">
-        <v>7.2690000000000001</v>
+        <v>7.6740000000000004</v>
       </c>
       <c r="I312" s="2">
-        <f t="shared" si="29"/>
-        <v>0.63689448287497885</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J312" s="2">
-        <f t="shared" si="29"/>
-        <v>1.0386225340486999</v>
-      </c>
-    </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
+        <f>(8*$E312*$D312*$C312*$C312)/(G312/1000)/10^12</f>
+        <v>0.63921320802641601</v>
+      </c>
+      <c r="K312" s="2">
+        <f>(8*$E312*$D312*$C312*$C312)/(H312/1000)/10^12</f>
+        <v>0.98380860046911645</v>
+      </c>
+      <c r="L312" s="2">
+        <f t="shared" si="31"/>
+        <v>6.681192212389381</v>
+      </c>
+      <c r="M312" s="2">
+        <f t="shared" si="30"/>
+        <v>20.614999999999998</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C313">
         <v>1536</v>
       </c>
@@ -13207,21 +13551,32 @@
         <v>50</v>
       </c>
       <c r="G313" s="2">
-        <v>22.073</v>
+        <v>21.866</v>
       </c>
       <c r="H313" s="2">
-        <v>9.3620000000000001</v>
+        <v>9.8859999999999992</v>
       </c>
       <c r="I313" s="2">
-        <f t="shared" ref="I313:J317" si="31">(8*$E313*$D313*$C313*$C313)/(G313/1000)/10^12</f>
-        <v>0.6840707833099261</v>
+        <v>1.89</v>
       </c>
       <c r="J313" s="2">
+        <f>(8*$E313*$D313*$C313*$C313)/(G313/1000)/10^12</f>
+        <v>0.69054671178999361</v>
+      </c>
+      <c r="K313" s="2">
+        <f>(8*$E313*$D313*$C313*$C313)/(H313/1000)/10^12</f>
+        <v>1.5273613594982804</v>
+      </c>
+      <c r="L313" s="2">
         <f t="shared" si="31"/>
-        <v>1.6128492202520828</v>
-      </c>
-    </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
+        <v>7.9891504761904768</v>
+      </c>
+      <c r="M313" s="2">
+        <f t="shared" si="30"/>
+        <v>33.641999999999996</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C314">
         <v>1536</v>
       </c>
@@ -13232,21 +13587,32 @@
         <v>50</v>
       </c>
       <c r="G314" s="2">
-        <v>11.577</v>
+        <v>11.811999999999999</v>
       </c>
       <c r="H314" s="2">
-        <v>31.28</v>
+        <v>31.908999999999999</v>
       </c>
       <c r="I314" s="2">
+        <v>3.1720000000000002</v>
+      </c>
+      <c r="J314" s="2">
+        <f>(8*$E314*$D314*$C314*$C314)/(G314/1000)/10^12</f>
+        <v>2.5566363697934307</v>
+      </c>
+      <c r="K314" s="2">
+        <f>(8*$E314*$D314*$C314*$C314)/(H314/1000)/10^12</f>
+        <v>0.94640975273433825</v>
+      </c>
+      <c r="L314" s="2">
         <f t="shared" si="31"/>
-        <v>2.6085331951282713</v>
-      </c>
-      <c r="J314" s="2">
-        <f t="shared" si="31"/>
-        <v>0.96544081841432217</v>
-      </c>
-    </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9.5204882723833535</v>
+      </c>
+      <c r="M314" s="2">
+        <f t="shared" si="30"/>
+        <v>46.892999999999994</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C315">
         <v>256</v>
       </c>
@@ -13257,21 +13623,32 @@
         <v>150</v>
       </c>
       <c r="G315" s="2">
-        <v>1.962</v>
+        <v>2.4529999999999998</v>
       </c>
       <c r="H315" s="2">
-        <v>3.6819999999999999</v>
+        <v>4.0590000000000002</v>
       </c>
       <c r="I315" s="2">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="J315" s="2">
+        <f>(8*$E315*$D315*$C315*$C315)/(G315/1000)/10^12</f>
+        <v>0.5129601304525071</v>
+      </c>
+      <c r="K315" s="2">
+        <f>(8*$E315*$D315*$C315*$C315)/(H315/1000)/10^12</f>
+        <v>0.31000029563932002</v>
+      </c>
+      <c r="L315" s="2">
         <f t="shared" si="31"/>
-        <v>0.64133088685015294</v>
-      </c>
-      <c r="J315" s="2">
-        <f t="shared" si="31"/>
-        <v>0.34174122759369907</v>
-      </c>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6.3230713567839185</v>
+      </c>
+      <c r="M315" s="2">
+        <f t="shared" si="30"/>
+        <v>6.7110000000000003</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C316">
         <v>256</v>
       </c>
@@ -13282,21 +13659,32 @@
         <v>150</v>
       </c>
       <c r="G316" s="2">
-        <v>6.6989999999999998</v>
+        <v>6.6070000000000002</v>
       </c>
       <c r="H316" s="2">
-        <v>15.285</v>
+        <v>15.624000000000001</v>
       </c>
       <c r="I316" s="2">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="J316" s="2">
+        <f>(8*$E316*$D316*$C316*$C316)/(G316/1000)/10^12</f>
+        <v>0.38089638262448922</v>
+      </c>
+      <c r="K316" s="2">
+        <f>(8*$E316*$D316*$C316*$C316)/(H316/1000)/10^12</f>
+        <v>0.16107158218125958</v>
+      </c>
+      <c r="L316" s="2">
         <f t="shared" si="31"/>
-        <v>0.37566538289296914</v>
-      </c>
-      <c r="J316" s="2">
-        <f t="shared" si="31"/>
-        <v>0.16464392541707557</v>
-      </c>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
+        <v>7.1291286118980173</v>
+      </c>
+      <c r="M316" s="2">
+        <f t="shared" si="30"/>
+        <v>22.584000000000003</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C317">
         <v>256</v>
       </c>
@@ -13307,34 +13695,45 @@
         <v>150</v>
       </c>
       <c r="G317" s="2">
-        <v>6.51</v>
+        <v>6.2590000000000003</v>
       </c>
       <c r="H317" s="2">
-        <v>9.0909999999999993</v>
+        <v>9.4909999999999997</v>
       </c>
       <c r="I317" s="2">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="J317" s="2">
+        <f>(8*$E317*$D317*$C317*$C317)/(G317/1000)/10^12</f>
+        <v>0.80414839431219032</v>
+      </c>
+      <c r="K317" s="2">
+        <f>(8*$E317*$D317*$C317*$C317)/(H317/1000)/10^12</f>
+        <v>0.53030921926035191</v>
+      </c>
+      <c r="L317" s="2">
         <f t="shared" si="31"/>
-        <v>0.77314359447004599</v>
-      </c>
-      <c r="J317" s="2">
-        <f t="shared" si="31"/>
-        <v>0.55364259157408424</v>
-      </c>
-    </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8.2241254901960783</v>
+      </c>
+      <c r="M317" s="2">
+        <f t="shared" si="30"/>
+        <v>16.361999999999998</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G318" s="2"/>
       <c r="H318" s="2"/>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G319" s="2"/>
       <c r="H319" s="2"/>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C320" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D320" t="s">
         <v>3</v>
@@ -13342,20 +13741,29 @@
       <c r="E320" t="s">
         <v>14</v>
       </c>
-      <c r="G320" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H320" s="2" t="s">
-        <v>20</v>
+      <c r="G320" t="s">
+        <v>17</v>
+      </c>
+      <c r="H320" t="s">
+        <v>77</v>
       </c>
       <c r="I320" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="J320" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="321" spans="3:10" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="K320" t="s">
+        <v>78</v>
+      </c>
+      <c r="L320" t="s">
+        <v>79</v>
+      </c>
+      <c r="M320" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="321" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C321">
         <v>2816</v>
       </c>
@@ -13366,21 +13774,32 @@
         <v>1500</v>
       </c>
       <c r="G321" s="2">
-        <v>592.91800000000001</v>
+        <v>643.70500000000004</v>
       </c>
       <c r="H321" s="2">
-        <v>1272.1690000000001</v>
+        <v>1319.0709999999999</v>
       </c>
       <c r="I321" s="2">
+        <v>233.00700000000001</v>
+      </c>
+      <c r="J321" s="2">
         <f>(6*$E321*$D321*$C321*$C321)/(G321/1000)/10^12</f>
-        <v>3.8517948991260171</v>
-      </c>
-      <c r="J321" s="2">
+        <v>3.5478962071135065</v>
+      </c>
+      <c r="K321" s="2">
         <f>(6*$E321*$D321*$C321*$C321)/(H321/1000)/10^12</f>
-        <v>1.7952005810548755</v>
-      </c>
-    </row>
-    <row r="322" spans="3:10" x14ac:dyDescent="0.2">
+        <v>1.7313689164571129</v>
+      </c>
+      <c r="L321" s="2">
+        <f>(6*$E321*$D321*$C321*$C321)/(I321/1000)/10^12</f>
+        <v>9.801415957460506</v>
+      </c>
+      <c r="M321" s="2">
+        <f>G321+H321+J321</f>
+        <v>1966.3238962071134</v>
+      </c>
+    </row>
+    <row r="322" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C322">
         <v>2816</v>
       </c>
@@ -13391,21 +13810,32 @@
         <v>750</v>
       </c>
       <c r="G322" s="2">
-        <v>298.53500000000003</v>
+        <v>332.334</v>
       </c>
       <c r="H322" s="2">
-        <v>638.21500000000003</v>
+        <v>656.85199999999998</v>
       </c>
       <c r="I322" s="2">
-        <f t="shared" ref="I322:I339" si="32">(6*$E322*$D322*$C322*$C322)/(G322/1000)/10^12</f>
-        <v>3.8250096772572726</v>
+        <v>113.032</v>
       </c>
       <c r="J322" s="2">
-        <f t="shared" ref="J322:J339" si="33">(6*$E322*$D322*$C322*$C322)/(H322/1000)/10^12</f>
-        <v>1.7892078124143118</v>
-      </c>
-    </row>
-    <row r="323" spans="3:10" x14ac:dyDescent="0.2">
+        <f>(6*$E322*$D322*$C322*$C322)/(G322/1000)/10^12</f>
+        <v>3.4359989167524234</v>
+      </c>
+      <c r="K322" s="2">
+        <f>(6*$E322*$D322*$C322*$C322)/(H322/1000)/10^12</f>
+        <v>1.7384422426969852</v>
+      </c>
+      <c r="L322" s="2">
+        <f t="shared" ref="L322:L339" si="32">(6*$E322*$D322*$C322*$C322)/(I322/1000)/10^12</f>
+        <v>10.102442352608112</v>
+      </c>
+      <c r="M322" s="2">
+        <f>G322+H322+J322</f>
+        <v>992.62199891675232</v>
+      </c>
+    </row>
+    <row r="323" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C323">
         <v>2816</v>
       </c>
@@ -13416,21 +13846,32 @@
         <v>375</v>
       </c>
       <c r="G323" s="2">
-        <v>150.70599999999999</v>
+        <v>170.238</v>
       </c>
       <c r="H323" s="2">
-        <v>319.88</v>
+        <v>331.95299999999997</v>
       </c>
       <c r="I323" s="2">
+        <v>59.963999999999999</v>
+      </c>
+      <c r="J323" s="2">
+        <f>(6*$E323*$D323*$C323*$C323)/(G323/1000)/10^12</f>
+        <v>3.3538318824234308</v>
+      </c>
+      <c r="K323" s="2">
+        <f>(6*$E323*$D323*$C323*$C323)/(H323/1000)/10^12</f>
+        <v>1.7199712971414629</v>
+      </c>
+      <c r="L323" s="2">
         <f t="shared" si="32"/>
-        <v>3.7884996748636421</v>
-      </c>
-      <c r="J323" s="2">
-        <f t="shared" si="33"/>
-        <v>1.7848869325997248</v>
-      </c>
-    </row>
-    <row r="324" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.5215401240744448</v>
+      </c>
+      <c r="M323" s="2">
+        <f>G323+H323+J323</f>
+        <v>505.54483188242341</v>
+      </c>
+    </row>
+    <row r="324" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C324">
         <v>2816</v>
       </c>
@@ -13441,21 +13882,32 @@
         <v>187</v>
       </c>
       <c r="G324" s="2">
-        <v>76.058999999999997</v>
+        <v>85.332999999999998</v>
       </c>
       <c r="H324" s="2">
-        <v>160.09399999999999</v>
+        <v>167.07599999999999</v>
       </c>
       <c r="I324" s="2">
+        <v>29.652999999999999</v>
+      </c>
+      <c r="J324" s="2">
+        <f>(6*$E324*$D324*$C324*$C324)/(G324/1000)/10^12</f>
+        <v>3.3364999452029109</v>
+      </c>
+      <c r="K324" s="2">
+        <f>(6*$E324*$D324*$C324*$C324)/(H324/1000)/10^12</f>
+        <v>1.704096039072039</v>
+      </c>
+      <c r="L324" s="2">
         <f t="shared" si="32"/>
-        <v>3.7433249164990339</v>
-      </c>
-      <c r="J324" s="2">
-        <f t="shared" si="33"/>
-        <v>1.7784148676652469</v>
-      </c>
-    </row>
-    <row r="325" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.6015091162445625</v>
+      </c>
+      <c r="M324" s="2">
+        <f>G324+H324+J324</f>
+        <v>255.74549994520291</v>
+      </c>
+    </row>
+    <row r="325" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C325">
         <v>2048</v>
       </c>
@@ -13466,21 +13918,32 @@
         <v>1500</v>
       </c>
       <c r="G325" s="2">
-        <v>396.38499999999999</v>
+        <v>420.95600000000002</v>
       </c>
       <c r="H325" s="2">
-        <v>927.20399999999995</v>
+        <v>939.24800000000005</v>
       </c>
       <c r="I325" s="2">
+        <v>120.626</v>
+      </c>
+      <c r="J325" s="2">
+        <f>(6*$E325*$D325*$C325*$C325)/(G325/1000)/10^12</f>
+        <v>2.8695625005938861</v>
+      </c>
+      <c r="K325" s="2">
+        <f>(6*$E325*$D325*$C325*$C325)/(H325/1000)/10^12</f>
+        <v>1.2860922269730677</v>
+      </c>
+      <c r="L325" s="2">
         <f t="shared" si="32"/>
-        <v>3.0474401200852705</v>
-      </c>
-      <c r="J325" s="2">
-        <f t="shared" si="33"/>
-        <v>1.3027980379722264</v>
-      </c>
-    </row>
-    <row r="326" spans="3:10" x14ac:dyDescent="0.2">
+        <v>10.014089433455473</v>
+      </c>
+      <c r="M325" s="2">
+        <f>G325+H325+J325</f>
+        <v>1363.0735625005941</v>
+      </c>
+    </row>
+    <row r="326" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C326">
         <v>2048</v>
       </c>
@@ -13491,21 +13954,32 @@
         <v>750</v>
       </c>
       <c r="G326" s="2">
-        <v>198.95500000000001</v>
+        <v>217.07400000000001</v>
       </c>
       <c r="H326" s="2">
-        <v>464.83199999999999</v>
+        <v>471.69400000000002</v>
       </c>
       <c r="I326" s="2">
+        <v>60.24</v>
+      </c>
+      <c r="J326" s="2">
+        <f>(6*$E326*$D326*$C326*$C326)/(G326/1000)/10^12</f>
+        <v>2.7823681140993393</v>
+      </c>
+      <c r="K326" s="2">
+        <f>(6*$E326*$D326*$C326*$C326)/(H326/1000)/10^12</f>
+        <v>1.2804482906290942</v>
+      </c>
+      <c r="L326" s="2">
         <f t="shared" si="32"/>
-        <v>3.0357607298132741</v>
-      </c>
-      <c r="J326" s="2">
-        <f t="shared" si="33"/>
-        <v>1.2993506815365552</v>
-      </c>
-    </row>
-    <row r="327" spans="3:10" x14ac:dyDescent="0.2">
+        <v>10.026224701195218</v>
+      </c>
+      <c r="M326" s="2">
+        <f>G326+H326+J326</f>
+        <v>691.55036811409934</v>
+      </c>
+    </row>
+    <row r="327" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C327">
         <v>2048</v>
       </c>
@@ -13516,21 +13990,32 @@
         <v>375</v>
       </c>
       <c r="G327" s="2">
-        <v>100.9</v>
+        <v>109.117</v>
       </c>
       <c r="H327" s="2">
-        <v>233.09200000000001</v>
+        <v>237.125</v>
       </c>
       <c r="I327" s="2">
+        <v>30.475999999999999</v>
+      </c>
+      <c r="J327" s="2">
+        <f>(6*$E327*$D327*$C327*$C327)/(G327/1000)/10^12</f>
+        <v>2.7675787274210251</v>
+      </c>
+      <c r="K327" s="2">
+        <f>(6*$E327*$D327*$C327*$C327)/(H327/1000)/10^12</f>
+        <v>1.2735472345809173</v>
+      </c>
+      <c r="L327" s="2">
         <f t="shared" si="32"/>
-        <v>2.9929622200198214</v>
-      </c>
-      <c r="J327" s="2">
-        <f t="shared" si="33"/>
-        <v>1.2955823794896435</v>
-      </c>
-    </row>
-    <row r="328" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.909105131907074</v>
+      </c>
+      <c r="M327" s="2">
+        <f>G327+H327+J327</f>
+        <v>349.00957872742106</v>
+      </c>
+    </row>
+    <row r="328" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C328">
         <v>2048</v>
       </c>
@@ -13541,21 +14026,32 @@
         <v>187</v>
       </c>
       <c r="G328" s="2">
-        <v>51.545000000000002</v>
+        <v>54.591999999999999</v>
       </c>
       <c r="H328" s="2">
-        <v>116.374</v>
+        <v>119.077</v>
       </c>
       <c r="I328" s="2">
+        <v>14.928000000000001</v>
+      </c>
+      <c r="J328" s="2">
+        <f>(6*$E328*$D328*$C328*$C328)/(G328/1000)/10^12</f>
+        <v>2.7585047409144194</v>
+      </c>
+      <c r="K328" s="2">
+        <f>(6*$E328*$D328*$C328*$C328)/(H328/1000)/10^12</f>
+        <v>1.264663123995398</v>
+      </c>
+      <c r="L328" s="2">
         <f t="shared" si="32"/>
-        <v>2.9215693242021534</v>
-      </c>
-      <c r="J328" s="2">
-        <f t="shared" si="33"/>
-        <v>1.2940372490075103</v>
-      </c>
-    </row>
-    <row r="329" spans="3:10" x14ac:dyDescent="0.2">
+        <v>10.087908012861737</v>
+      </c>
+      <c r="M328" s="2">
+        <f>G328+H328+J328</f>
+        <v>176.4275047409144</v>
+      </c>
+    </row>
+    <row r="329" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C329">
         <v>1536</v>
       </c>
@@ -13566,21 +14062,32 @@
         <v>1500</v>
       </c>
       <c r="G329" s="2">
-        <v>296.66699999999997</v>
+        <v>308.45400000000001</v>
       </c>
       <c r="H329" s="2">
-        <v>694.33199999999999</v>
+        <v>704.15099999999995</v>
       </c>
       <c r="I329" s="2">
+        <v>69.688000000000002</v>
+      </c>
+      <c r="J329" s="2">
+        <f>(6*$E329*$D329*$C329*$C329)/(G329/1000)/10^12</f>
+        <v>2.2028479060086754</v>
+      </c>
+      <c r="K329" s="2">
+        <f>(6*$E329*$D329*$C329*$C329)/(H329/1000)/10^12</f>
+        <v>0.96495957259167431</v>
+      </c>
+      <c r="L329" s="2">
         <f t="shared" si="32"/>
-        <v>2.2903701726177839</v>
-      </c>
-      <c r="J329" s="2">
-        <f t="shared" si="33"/>
-        <v>0.97860569295380306</v>
-      </c>
-    </row>
-    <row r="330" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.7502762025025813</v>
+      </c>
+      <c r="M329" s="2">
+        <f>G329+H329+J329</f>
+        <v>1014.8078479060086</v>
+      </c>
+    </row>
+    <row r="330" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C330">
         <v>1536</v>
       </c>
@@ -13591,21 +14098,32 @@
         <v>750</v>
       </c>
       <c r="G330" s="2">
-        <v>149.95599999999999</v>
+        <v>153.66</v>
       </c>
       <c r="H330" s="2">
-        <v>348.52300000000002</v>
+        <v>353.55399999999997</v>
       </c>
       <c r="I330" s="2">
+        <v>34.82</v>
+      </c>
+      <c r="J330" s="2">
+        <f>(6*$E330*$D330*$C330*$C330)/(G330/1000)/10^12</f>
+        <v>2.2109763373682156</v>
+      </c>
+      <c r="K330" s="2">
+        <f>(6*$E330*$D330*$C330*$C330)/(H330/1000)/10^12</f>
+        <v>0.9609242831363809</v>
+      </c>
+      <c r="L330" s="2">
         <f t="shared" si="32"/>
-        <v>2.2655887326949244</v>
-      </c>
-      <c r="J330" s="2">
-        <f t="shared" si="33"/>
-        <v>0.97479541952754911</v>
-      </c>
-    </row>
-    <row r="331" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.756996668581273</v>
+      </c>
+      <c r="M330" s="2">
+        <f>G330+H330+J330</f>
+        <v>509.42497633736815</v>
+      </c>
+    </row>
+    <row r="331" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C331">
         <v>1536</v>
       </c>
@@ -13616,21 +14134,32 @@
         <v>375</v>
       </c>
       <c r="G331" s="2">
-        <v>76.866</v>
+        <v>78.302000000000007</v>
       </c>
       <c r="H331" s="2">
-        <v>175.45500000000001</v>
+        <v>178.547</v>
       </c>
       <c r="I331" s="2">
+        <v>17.274000000000001</v>
+      </c>
+      <c r="J331" s="2">
+        <f>(6*$E331*$D331*$C331*$C331)/(G331/1000)/10^12</f>
+        <v>2.1694121733799898</v>
+      </c>
+      <c r="K331" s="2">
+        <f>(6*$E331*$D331*$C331*$C331)/(H331/1000)/10^12</f>
+        <v>0.95139829848723312</v>
+      </c>
+      <c r="L331" s="2">
         <f t="shared" si="32"/>
-        <v>2.2099408320974159</v>
-      </c>
-      <c r="J331" s="2">
-        <f t="shared" si="33"/>
-        <v>0.96816455501410625</v>
-      </c>
-    </row>
-    <row r="332" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.8338145189301844</v>
+      </c>
+      <c r="M331" s="2">
+        <f>G331+H331+J331</f>
+        <v>259.01841217338</v>
+      </c>
+    </row>
+    <row r="332" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C332">
         <v>1536</v>
       </c>
@@ -13641,21 +14170,32 @@
         <v>187</v>
       </c>
       <c r="G332" s="2">
-        <v>39.563000000000002</v>
+        <v>40.225000000000001</v>
       </c>
       <c r="H332" s="2">
-        <v>88.668000000000006</v>
+        <v>90.17</v>
       </c>
       <c r="I332" s="2">
+        <v>8.5850000000000009</v>
+      </c>
+      <c r="J332" s="2">
+        <f>(6*$E332*$D332*$C332*$C332)/(G332/1000)/10^12</f>
+        <v>2.105858634779366</v>
+      </c>
+      <c r="K332" s="2">
+        <f>(6*$E332*$D332*$C332*$C332)/(H332/1000)/10^12</f>
+        <v>0.93942734372851278</v>
+      </c>
+      <c r="L332" s="2">
         <f t="shared" si="32"/>
-        <v>2.1410955585774589</v>
-      </c>
-      <c r="J332" s="2">
-        <f t="shared" si="33"/>
-        <v>0.95534086236297189</v>
-      </c>
-    </row>
-    <row r="333" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.8669963405940582</v>
+      </c>
+      <c r="M332" s="2">
+        <f>G332+H332+J332</f>
+        <v>132.50085863477938</v>
+      </c>
+    </row>
+    <row r="333" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C333">
         <v>2560</v>
       </c>
@@ -13666,21 +14206,32 @@
         <v>1500</v>
       </c>
       <c r="G333" s="2">
-        <v>522.601</v>
+        <v>583.35799999999995</v>
       </c>
       <c r="H333" s="2">
-        <v>1154.9090000000001</v>
+        <v>1190.5219999999999</v>
       </c>
       <c r="I333" s="2">
+        <v>198.49299999999999</v>
+      </c>
+      <c r="J333" s="2">
+        <f>(6*$E333*$D333*$C333*$C333)/(G333/1000)/10^12</f>
+        <v>3.2354691287339854</v>
+      </c>
+      <c r="K333" s="2">
+        <f>(6*$E333*$D333*$C333*$C333)/(H333/1000)/10^12</f>
+        <v>1.5853859063503237</v>
+      </c>
+      <c r="L333" s="2">
         <f t="shared" si="32"/>
-        <v>3.6116211029064238</v>
-      </c>
-      <c r="J333" s="2">
-        <f t="shared" si="33"/>
-        <v>1.6342731765013518</v>
-      </c>
-    </row>
-    <row r="334" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.5088330570851376</v>
+      </c>
+      <c r="M333" s="2">
+        <f>G333+H333+J333</f>
+        <v>1777.1154691287338</v>
+      </c>
+    </row>
+    <row r="334" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C334">
         <v>2560</v>
       </c>
@@ -13691,21 +14242,32 @@
         <v>750</v>
       </c>
       <c r="G334" s="2">
-        <v>263.452</v>
+        <v>302.53699999999998</v>
       </c>
       <c r="H334" s="2">
-        <v>579.39599999999996</v>
+        <v>596.52099999999996</v>
       </c>
       <c r="I334" s="2">
+        <v>94.861000000000004</v>
+      </c>
+      <c r="J334" s="2">
+        <f>(6*$E334*$D334*$C334*$C334)/(G334/1000)/10^12</f>
+        <v>3.1193487077613646</v>
+      </c>
+      <c r="K334" s="2">
+        <f>(6*$E334*$D334*$C334*$C334)/(H334/1000)/10^12</f>
+        <v>1.5820371789090411</v>
+      </c>
+      <c r="L334" s="2">
         <f t="shared" si="32"/>
-        <v>3.5821265353840546</v>
-      </c>
-      <c r="J334" s="2">
-        <f t="shared" si="33"/>
-        <v>1.6287968850319989</v>
-      </c>
-    </row>
-    <row r="335" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.948434024520088</v>
+      </c>
+      <c r="M334" s="2">
+        <f>G334+H334+J334</f>
+        <v>902.17734870776133</v>
+      </c>
+    </row>
+    <row r="335" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C335">
         <v>2560</v>
       </c>
@@ -13716,21 +14278,32 @@
         <v>375</v>
       </c>
       <c r="G335" s="2">
-        <v>132.929</v>
+        <v>153.83699999999999</v>
       </c>
       <c r="H335" s="2">
-        <v>290.43200000000002</v>
+        <v>299.49099999999999</v>
       </c>
       <c r="I335" s="2">
+        <v>47.874000000000002</v>
+      </c>
+      <c r="J335" s="2">
+        <f>(6*$E335*$D335*$C335*$C335)/(G335/1000)/10^12</f>
+        <v>3.0672673024044932</v>
+      </c>
+      <c r="K335" s="2">
+        <f>(6*$E335*$D335*$C335*$C335)/(H335/1000)/10^12</f>
+        <v>1.5755371613838145</v>
+      </c>
+      <c r="L335" s="2">
         <f t="shared" si="32"/>
-        <v>3.5497084909989547</v>
-      </c>
-      <c r="J335" s="2">
-        <f t="shared" si="33"/>
-        <v>1.6246804759806082</v>
-      </c>
-    </row>
-    <row r="336" spans="3:10" x14ac:dyDescent="0.2">
+        <v>9.8562727158791841</v>
+      </c>
+      <c r="M335" s="2">
+        <f>G335+H335+J335</f>
+        <v>456.39526730240448</v>
+      </c>
+    </row>
+    <row r="336" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C336">
         <v>2560</v>
       </c>
@@ -13741,21 +14314,32 @@
         <v>187</v>
       </c>
       <c r="G336" s="2">
-        <v>67.132000000000005</v>
+        <v>77.613</v>
       </c>
       <c r="H336" s="2">
-        <v>145.24199999999999</v>
+        <v>150.583</v>
       </c>
       <c r="I336" s="2">
+        <v>23.888000000000002</v>
+      </c>
+      <c r="J336" s="2">
+        <f>(6*$E336*$D336*$C336*$C336)/(G336/1000)/10^12</f>
+        <v>3.0317144602064086</v>
+      </c>
+      <c r="K336" s="2">
+        <f>(6*$E336*$D336*$C336*$C336)/(H336/1000)/10^12</f>
+        <v>1.5625964046406302</v>
+      </c>
+      <c r="L336" s="2">
         <f t="shared" si="32"/>
-        <v>3.5050416254543282</v>
-      </c>
-      <c r="J336" s="2">
-        <f t="shared" si="33"/>
-        <v>1.6200579336555545</v>
-      </c>
-    </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
+        <v>9.85015298057602</v>
+      </c>
+      <c r="M336" s="2">
+        <f>G336+H336+J336</f>
+        <v>231.22771446020641</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C337">
         <v>512</v>
       </c>
@@ -13766,21 +14350,32 @@
         <v>1</v>
       </c>
       <c r="G337" s="2">
-        <v>0.11600000000000001</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="H337" s="2">
-        <v>0.17599999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="I337" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="J337" s="2">
+        <f>(6*$E337*$D337*$C337*$C337)/(G337/1000)/10^12</f>
+        <v>0.66225852631578941</v>
+      </c>
+      <c r="K337" s="2">
+        <f>(6*$E337*$D337*$C337*$C337)/(H337/1000)/10^12</f>
+        <v>0.23967451428571429</v>
+      </c>
+      <c r="L337" s="2">
         <f t="shared" si="32"/>
-        <v>0.43389351724137931</v>
-      </c>
-      <c r="J337" s="2">
-        <f t="shared" si="33"/>
-        <v>0.28597527272727269</v>
-      </c>
-    </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1.3603148108108107</v>
+      </c>
+      <c r="M337" s="2">
+        <f>G337+H337+J337</f>
+        <v>0.94825852631578944</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C338">
         <v>1024</v>
       </c>
@@ -13791,21 +14386,32 @@
         <v>1500</v>
       </c>
       <c r="G338" s="2">
-        <v>179.69399999999999</v>
+        <v>189.238</v>
       </c>
       <c r="H338" s="2">
-        <v>469.43200000000002</v>
+        <v>477.36399999999998</v>
       </c>
       <c r="I338" s="2">
+        <v>32.561999999999998</v>
+      </c>
+      <c r="J338" s="2">
+        <f>(6*$E338*$D338*$C338*$C338)/(G338/1000)/10^12</f>
+        <v>1.5958205434426489</v>
+      </c>
+      <c r="K338" s="2">
+        <f>(6*$E338*$D338*$C338*$C338)/(H338/1000)/10^12</f>
+        <v>0.63261973672082528</v>
+      </c>
+      <c r="L338" s="2">
         <f t="shared" si="32"/>
-        <v>1.6805785835921068</v>
-      </c>
-      <c r="J338" s="2">
-        <f t="shared" si="33"/>
-        <v>0.64330912251401695</v>
-      </c>
-    </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
+        <v>9.2743040353786625</v>
+      </c>
+      <c r="M338" s="2">
+        <f>G338+H338+J338</f>
+        <v>668.19782054344262</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C339">
         <v>1024</v>
       </c>
@@ -13816,53 +14422,64 @@
         <v>1500</v>
       </c>
       <c r="G339" s="2">
-        <v>210.16399999999999</v>
+        <v>218.98</v>
       </c>
       <c r="H339" s="2">
-        <v>175.30799999999999</v>
+        <v>181.887</v>
       </c>
       <c r="I339" s="2">
+        <v>68.981999999999999</v>
+      </c>
+      <c r="J339" s="2">
+        <f>(6*$E339*$D339*$C339*$C339)/(G339/1000)/10^12</f>
+        <v>2.7581504064298112</v>
+      </c>
+      <c r="K339" s="2">
+        <f>(6*$E339*$D339*$C339*$C339)/(H339/1000)/10^12</f>
+        <v>3.3206319088225107</v>
+      </c>
+      <c r="L339" s="2">
         <f t="shared" si="32"/>
-        <v>2.8738498315601153</v>
-      </c>
-      <c r="J339" s="2">
-        <f t="shared" si="33"/>
-        <v>3.4452493668286674</v>
-      </c>
-    </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+        <v>8.7556141602157087</v>
+      </c>
+      <c r="M339" s="2">
+        <f>G339+H339+J339</f>
+        <v>403.62515040642978</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I340" s="3"/>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G341" s="2"/>
       <c r="H341" s="2"/>
       <c r="I341" s="2"/>
       <c r="K341" s="2"/>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
+        <v>65</v>
+      </c>
+      <c r="C342" t="s">
+        <v>66</v>
+      </c>
+      <c r="D342" t="s">
+        <v>67</v>
+      </c>
+      <c r="G342" t="s">
+        <v>68</v>
+      </c>
+      <c r="I342" t="s">
         <v>69</v>
       </c>
-      <c r="C342" t="s">
+      <c r="J342" t="s">
         <v>70</v>
       </c>
-      <c r="D342" t="s">
+      <c r="K342" t="s">
         <v>71</v>
       </c>
-      <c r="G342" t="s">
-        <v>72</v>
-      </c>
-      <c r="I342" t="s">
-        <v>73</v>
-      </c>
-      <c r="J342" t="s">
-        <v>74</v>
-      </c>
-      <c r="K342" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C344">
         <v>100000</v>
       </c>
@@ -13877,13 +14494,13 @@
         <v>12.929842512901963</v>
       </c>
       <c r="J344" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K344" s="2">
         <v>2.7217404818666263E-3</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C345">
         <v>100000</v>
       </c>
@@ -13898,13 +14515,13 @@
         <v>17.447016273977042</v>
       </c>
       <c r="J345" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K345" s="2">
         <v>2.8143182937997221E-3</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C346">
         <v>100000</v>
       </c>
@@ -13919,13 +14536,13 @@
         <v>21.30019023732406</v>
       </c>
       <c r="J346" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K346" s="2">
         <v>3.0198935219988374E-3</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C347">
         <v>100000</v>
       </c>
@@ -13942,13 +14559,13 @@
         <v>12.952755734200144</v>
       </c>
       <c r="J347" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K347" s="2">
         <v>1.4072668142911852E-2</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C348">
         <v>100000</v>
       </c>
@@ -13965,13 +14582,13 @@
         <v>17.14457619277362</v>
       </c>
       <c r="J348" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K348" s="2">
         <v>1.2046923143319737E-2</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C349">
         <v>3097600</v>
       </c>
@@ -13986,13 +14603,13 @@
         <v>23.881655664241311</v>
       </c>
       <c r="J349" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K349" s="2">
         <v>1.4244112357114759E-3</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C350">
         <v>3097600</v>
       </c>
@@ -14007,13 +14624,13 @@
         <v>29.671386236417515</v>
       </c>
       <c r="J350" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K350" s="2">
         <v>2.5396850198400474E-3</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C351">
         <v>3097600</v>
       </c>
@@ -14028,13 +14645,13 @@
         <v>39.892006905215467</v>
       </c>
       <c r="J351" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K351" s="2">
         <v>3.6299779251177419E-3</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C352">
         <v>3097600</v>
       </c>
@@ -14051,7 +14668,7 @@
         <v>47.42458307771637</v>
       </c>
       <c r="J352" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K352" s="2">
         <v>8.2743340547744307E-2</v>
@@ -14074,7 +14691,7 @@
         <v>85.433220551533722</v>
       </c>
       <c r="J353" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K353" s="2">
         <v>0.13990011861380916</v>
@@ -14095,7 +14712,7 @@
         <v>24.034404412291384</v>
       </c>
       <c r="J354" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K354" s="2">
         <v>1.5525869752736773E-3</v>
@@ -14116,7 +14733,7 @@
         <v>29.729046891266307</v>
       </c>
       <c r="J355" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K355" s="2">
         <v>3.2811262507992625E-3</v>
@@ -14137,7 +14754,7 @@
         <v>39.848130391275063</v>
       </c>
       <c r="J356" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K356" s="2">
         <v>4.2892095640351307E-3</v>
@@ -14160,7 +14777,7 @@
         <v>47.673587747730288</v>
       </c>
       <c r="J357" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K357" s="2">
         <v>2.016955508603064E-2</v>
@@ -14183,7 +14800,7 @@
         <v>91.739442108874087</v>
       </c>
       <c r="J358" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K358" s="2">
         <v>1.7192171987028774E-2</v>
@@ -14204,7 +14821,7 @@
         <v>24.144603836146352</v>
       </c>
       <c r="J359" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K359" s="2">
         <v>2.3946211655115719E-3</v>
@@ -14225,7 +14842,7 @@
         <v>29.947763005697809</v>
       </c>
       <c r="J360" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K360" s="2">
         <v>3.9639825800243155E-3</v>
@@ -14246,7 +14863,7 @@
         <v>39.96287932923633</v>
       </c>
       <c r="J361" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K361" s="2">
         <v>5.9989034085624502E-3</v>
@@ -14269,7 +14886,7 @@
         <v>47.303778546843922</v>
       </c>
       <c r="J362" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K362" s="2">
         <v>2.8287996077934911E-2</v>
@@ -14292,7 +14909,7 @@
         <v>93.278211847953969</v>
       </c>
       <c r="J363" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K363" s="2">
         <v>2.8402430673410639E-2</v>
@@ -14313,7 +14930,7 @@
         <v>24.364903923828887</v>
       </c>
       <c r="J364" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K364" s="2">
         <v>5.5086057076273323E-3</v>
@@ -14334,7 +14951,7 @@
         <v>29.908576521971654</v>
       </c>
       <c r="J365" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K365" s="2">
         <v>6.9175596548888335E-3</v>
@@ -14355,7 +14972,7 @@
         <v>39.993810419514524</v>
       </c>
       <c r="J366" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K366" s="2">
         <v>1.620355711434673E-2</v>
@@ -14379,7 +14996,7 @@
         <v>19.024424073809129</v>
       </c>
       <c r="J367" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K367" s="2">
         <v>0.14542319323814551</v>
@@ -14403,7 +15020,7 @@
         <v>34.741025289475012</v>
       </c>
       <c r="J368" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K368" s="2">
         <v>0.11239437837131218</v>
@@ -14423,7 +15040,7 @@
         <v>24.469064828510039</v>
       </c>
       <c r="J369" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K369" s="2">
         <v>1.1203735279384621E-2</v>
@@ -14443,7 +15060,7 @@
         <v>30.008238380094905</v>
       </c>
       <c r="J370" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K370" s="2">
         <v>1.4427586879236077E-2</v>
@@ -14463,7 +15080,7 @@
         <v>40.182660359755808</v>
       </c>
       <c r="J371" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K371" s="2">
         <v>2.5303421861375297E-2</v>
@@ -14486,7 +15103,7 @@
         <v>47.263142838056389</v>
       </c>
       <c r="J372" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K372" s="2">
         <v>0.12958876291439875</v>
@@ -14509,7 +15126,7 @@
         <v>85.52970680510991</v>
       </c>
       <c r="J373" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K373" s="2">
         <v>0.1155943219330338</v>
@@ -14529,7 +15146,7 @@
         <v>24.484218118321408</v>
       </c>
       <c r="J374" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K374" s="2">
         <v>1.6054512400601084E-2</v>
@@ -14549,7 +15166,7 @@
         <v>29.97477413630099</v>
       </c>
       <c r="J375" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K375" s="2">
         <v>2.9023538541564975E-2</v>
@@ -14569,7 +15186,7 @@
         <v>40.241174090844822</v>
       </c>
       <c r="J376" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K376" s="2">
         <v>3.3668468772335348E-2</v>
@@ -14592,7 +15209,7 @@
         <v>47.193900737096016</v>
       </c>
       <c r="J377" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K377" s="2">
         <v>0.22045191169146514</v>
@@ -14615,7 +15232,7 @@
         <v>84.820086333409833</v>
       </c>
       <c r="J378" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K378" s="2">
         <v>0.25675923859768651</v>
@@ -14628,7 +15245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14642,31 +15259,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4" s="8">
         <v>8</v>
@@ -14674,7 +15291,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B5" s="8">
         <v>5</v>
@@ -14682,15 +15299,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9">
         <v>367.48</v>
@@ -14698,26 +15315,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>